<commit_message>
Update cralwer and partial NAV files download
</commit_message>
<xml_diff>
--- a/Individual Homework/IHW01/ETF_Vol_Alt_Group16.xlsx
+++ b/Individual Homework/IHW01/ETF_Vol_Alt_Group16.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="117">
   <si>
+    <t>ETF Name</t>
+  </si>
+  <si>
+    <t>Asset Class</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>Issuer</t>
+  </si>
+  <si>
     <t>Symbol</t>
-  </si>
-  <si>
-    <t>ETF Name</t>
-  </si>
-  <si>
-    <t>Asset Class</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>Issuer</t>
   </si>
   <si>
     <t>QAI</t>
@@ -735,13 +735,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,705 +757,603 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0</v>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>4</v>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>5</v>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>6</v>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>10</v>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>11</v>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1">
-        <v>13</v>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>14</v>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1">
-        <v>15</v>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1">
-        <v>16</v>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1">
-        <v>17</v>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1">
-        <v>18</v>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1">
-        <v>19</v>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1">
-        <v>20</v>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1">
-        <v>21</v>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E23" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1">
-        <v>22</v>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F24" t="s">
+      <c r="E24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1">
-        <v>23</v>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F25" t="s">
+      <c r="E25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1">
-        <v>24</v>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F26" t="s">
+      <c r="E26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1">
-        <v>25</v>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F27" t="s">
+      <c r="E27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1">
-        <v>26</v>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="1">
-        <v>27</v>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F29" t="s">
+      <c r="E29" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1">
-        <v>28</v>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F30" t="s">
+      <c r="E30" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1">
-        <v>29</v>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F31" t="s">
+      <c r="E31" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1">
-        <v>30</v>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F32" t="s">
+      <c r="E32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1">
-        <v>31</v>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F33" t="s">
+      <c r="E33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="1">
-        <v>32</v>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F34" t="s">
+      <c r="E34" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E31" r:id="rId30"/>
-    <hyperlink ref="E32" r:id="rId31"/>
-    <hyperlink ref="E33" r:id="rId32"/>
-    <hyperlink ref="E34" r:id="rId33"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>